<commit_message>
Help ins Englische übersetzt
</commit_message>
<xml_diff>
--- a/Ausarbeitung/Zeitmessungen.xlsx
+++ b/Ausarbeitung/Zeitmessungen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Grad 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="20">
   <si>
     <t xml:space="preserve">ZEIT ( in Nanosekunden)</t>
   </si>
@@ -84,10 +84,7 @@
     <t xml:space="preserve">Linux Kernel 5.4.0-26-generic</t>
   </si>
   <si>
-    <t xml:space="preserve">Kompiliert mit Option -03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gcc version adden</t>
+    <t xml:space="preserve">Kompiliert mit GCC 9.3.0 mit Option -03</t>
   </si>
   <si>
     <t xml:space="preserve">ZEIT ( in Sekunden)</t>
@@ -103,7 +100,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,12 +130,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,7 +174,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -224,10 +215,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,14 +227,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{40131631-FC7F-0000-9F42-96F1177F0000}"/>
-</file>
-
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -256,10 +235,10 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.15"/>
@@ -792,7 +771,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>13</v>
       </c>
@@ -800,31 +779,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
@@ -847,10 +822,10 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.15"/>
@@ -1379,7 +1354,7 @@
         <v>5858</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>13</v>
       </c>
@@ -1387,31 +1362,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
@@ -1434,10 +1405,10 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.15"/>
@@ -1445,7 +1416,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.15"/>
   </cols>
   <sheetData>
@@ -1505,11 +1477,11 @@
       </c>
       <c r="K4" s="1" t="n">
         <f aca="false">AVERAGE(D:D)</f>
-        <v>24362.05</v>
+        <v>21693.7</v>
       </c>
       <c r="L4" s="1" t="n">
         <f aca="false">AVERAGE(E:E)</f>
-        <v>21685.7</v>
+        <v>22095.6</v>
       </c>
       <c r="M4" s="1" t="n">
         <f aca="false">AVERAGE(F:F)</f>
@@ -1548,7 +1520,7 @@
       </c>
       <c r="K5" s="1" t="n">
         <f aca="false">MAX(D:D)</f>
-        <v>29460</v>
+        <v>22910</v>
       </c>
       <c r="L5" s="1" t="n">
         <f aca="false">MAX(E:E)</f>
@@ -1595,7 +1567,7 @@
       </c>
       <c r="L6" s="1" t="n">
         <f aca="false">MIN(E:E)</f>
-        <v>18577</v>
+        <v>18616</v>
       </c>
       <c r="M6" s="1" t="n">
         <f aca="false">MIN(F:F)</f>
@@ -1654,10 +1626,10 @@
         <v>22835</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>27892</v>
+        <v>21174</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>18794</v>
+        <v>23487</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>35212</v>
@@ -1674,7 +1646,7 @@
         <v>32542</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>28969</v>
+        <v>21860</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>19659</v>
@@ -1694,7 +1666,7 @@
         <v>32308</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>26652</v>
+        <v>21583</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>24683</v>
@@ -1717,7 +1689,7 @@
         <v>22910</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>18577</v>
+        <v>22082</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>25988</v>
@@ -1774,7 +1746,7 @@
         <v>34126</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>29460</v>
+        <v>21810</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>19575</v>
@@ -1794,7 +1766,7 @@
         <v>23261</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>26341</v>
+        <v>22650</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>26325</v>
@@ -1806,7 +1778,7 @@
         <v>24331</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
         <v>13</v>
       </c>
@@ -1814,7 +1786,7 @@
         <v>32492</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>26323</v>
+        <v>21359</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>20154</v>
@@ -1874,7 +1846,7 @@
         <v>23479</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>28255</v>
+        <v>21702</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>26268</v>
@@ -1894,7 +1866,7 @@
         <v>22470</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>27967</v>
+        <v>22466</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>18616</v>
@@ -1914,7 +1886,7 @@
         <v>23098</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>27362</v>
+        <v>21250</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>19103</v>
@@ -1966,7 +1938,7 @@
         <v>18363</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>13</v>
       </c>
@@ -1974,31 +1946,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
@@ -2020,11 +1988,11 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.15"/>
@@ -2553,7 +2521,7 @@
         <v>213572</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>13</v>
       </c>
@@ -2561,31 +2529,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
@@ -2607,11 +2571,11 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.15"/>
@@ -3139,7 +3103,7 @@
         <v>1880370</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>13</v>
       </c>
@@ -3147,31 +3111,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
@@ -3193,11 +3153,11 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.15"/>
@@ -3725,7 +3685,7 @@
         <v>5968152</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>13</v>
       </c>
@@ -3733,31 +3693,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
@@ -3779,11 +3735,11 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.15"/>
@@ -4315,7 +4271,7 @@
         <v>31633687</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>13</v>
       </c>
@@ -4323,31 +4279,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
@@ -4369,11 +4321,11 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="25.15"/>
@@ -4393,7 +4345,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -4655,7 +4607,7 @@
       <c r="B12" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="8" t="n">
         <v>0.316063</v>
       </c>
       <c r="D12" s="6" t="n">
@@ -4912,7 +4864,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>13</v>
       </c>
@@ -4920,31 +4872,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
@@ -4966,21 +4914,21 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="13.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="6" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.57"/>
@@ -4988,18 +4936,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="C1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -5015,7 +4963,7 @@
         <v>6</v>
       </c>
       <c r="J3" s="3"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -5038,9 +4986,9 @@
       <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="K4" s="5" t="n">
         <f aca="false">AVERAGE(C:C)</f>
-        <v>375280389.65</v>
+        <v>2.81628035</v>
       </c>
       <c r="L4" s="5" t="n">
         <f aca="false">AVERAGE(D:D)</f>
@@ -5063,8 +5011,8 @@
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>374294983</v>
+      <c r="C5" s="5" t="n">
+        <v>2.974295</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>2.402683</v>
@@ -5082,9 +5030,9 @@
       <c r="J5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="K5" s="5" t="n">
         <f aca="false">MAX(C:C)</f>
-        <v>401849698</v>
+        <v>2.993177</v>
       </c>
       <c r="L5" s="5" t="n">
         <f aca="false">MAX(D:D)</f>
@@ -5107,8 +5055,8 @@
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>369115781</v>
+      <c r="C6" s="5" t="n">
+        <v>2.969116</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>2.397129</v>
@@ -5126,9 +5074,9 @@
       <c r="J6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="K6" s="5" t="n">
         <f aca="false">MIN(C:C)</f>
-        <v>365116340</v>
+        <v>2.667663</v>
       </c>
       <c r="L6" s="5" t="n">
         <f aca="false">MIN(D:D)</f>
@@ -5151,8 +5099,8 @@
       <c r="B7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>365361590</v>
+      <c r="C7" s="5" t="n">
+        <v>2.815362</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>2.408448</v>
@@ -5171,8 +5119,8 @@
       <c r="B8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>369738954</v>
+      <c r="C8" s="5" t="n">
+        <v>2.669739</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>2.403862</v>
@@ -5191,8 +5139,8 @@
       <c r="B9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>384714342</v>
+      <c r="C9" s="5" t="n">
+        <v>2.834714</v>
       </c>
       <c r="D9" s="6" t="n">
         <v>2.399091</v>
@@ -5211,8 +5159,8 @@
       <c r="B10" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>379622389</v>
+      <c r="C10" s="5" t="n">
+        <v>2.749622</v>
       </c>
       <c r="D10" s="6" t="n">
         <v>2.402336</v>
@@ -5231,8 +5179,8 @@
       <c r="B11" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="n">
-        <v>370558451</v>
+      <c r="C11" s="5" t="n">
+        <v>2.740558</v>
       </c>
       <c r="D11" s="6" t="n">
         <v>2.402084</v>
@@ -5251,8 +5199,8 @@
       <c r="B12" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C12" s="1" t="n">
-        <v>370085855</v>
+      <c r="C12" s="5" t="n">
+        <v>2.970086</v>
       </c>
       <c r="D12" s="6" t="n">
         <v>2.426171</v>
@@ -5271,8 +5219,8 @@
       <c r="B13" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C13" s="1" t="n">
-        <v>368458274</v>
+      <c r="C13" s="5" t="n">
+        <v>2.668458</v>
       </c>
       <c r="D13" s="6" t="n">
         <v>2.401036</v>
@@ -5291,8 +5239,8 @@
       <c r="B14" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>366311159</v>
+      <c r="C14" s="5" t="n">
+        <v>2.966311</v>
       </c>
       <c r="D14" s="6" t="n">
         <v>2.403934</v>
@@ -5311,8 +5259,8 @@
       <c r="B15" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="1" t="n">
-        <v>394321048</v>
+      <c r="C15" s="5" t="n">
+        <v>2.764321</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>2.400091</v>
@@ -5331,8 +5279,8 @@
       <c r="B16" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="1" t="n">
-        <v>365116340</v>
+      <c r="C16" s="5" t="n">
+        <v>2.735116</v>
       </c>
       <c r="D16" s="6" t="n">
         <v>2.411055</v>
@@ -5351,8 +5299,8 @@
       <c r="B17" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="1" t="n">
-        <v>367981460</v>
+      <c r="C17" s="5" t="n">
+        <v>2.817981</v>
       </c>
       <c r="D17" s="6" t="n">
         <v>2.399408</v>
@@ -5371,8 +5319,8 @@
       <c r="B18" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="n">
-        <v>367823709</v>
+      <c r="C18" s="5" t="n">
+        <v>2.737824</v>
       </c>
       <c r="D18" s="6" t="n">
         <v>2.396975</v>
@@ -5391,8 +5339,8 @@
       <c r="B19" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>367662805</v>
+      <c r="C19" s="5" t="n">
+        <v>2.667663</v>
       </c>
       <c r="D19" s="6" t="n">
         <v>2.405839</v>
@@ -5411,8 +5359,8 @@
       <c r="B20" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C20" s="1" t="n">
-        <v>393176757</v>
+      <c r="C20" s="5" t="n">
+        <v>2.993177</v>
       </c>
       <c r="D20" s="6" t="n">
         <v>2.454965</v>
@@ -5431,8 +5379,8 @@
       <c r="B21" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>369549230</v>
+      <c r="C21" s="5" t="n">
+        <v>2.969549</v>
       </c>
       <c r="D21" s="6" t="n">
         <v>2.400499</v>
@@ -5451,8 +5399,8 @@
       <c r="B22" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="1" t="n">
-        <v>401849698</v>
+      <c r="C22" s="5" t="n">
+        <v>2.77185</v>
       </c>
       <c r="D22" s="6" t="n">
         <v>2.408389</v>
@@ -5471,8 +5419,8 @@
       <c r="B23" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>377499437</v>
+      <c r="C23" s="5" t="n">
+        <v>2.827499</v>
       </c>
       <c r="D23" s="6" t="n">
         <v>2.418307</v>
@@ -5491,8 +5439,8 @@
       <c r="B24" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>382365531</v>
+      <c r="C24" s="5" t="n">
+        <v>2.682366</v>
       </c>
       <c r="D24" s="6" t="n">
         <v>2.409406</v>
@@ -5535,11 +5483,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>

</xml_diff>

<commit_message>
dezimalzahlen jetzt mit komma angegeben
</commit_message>
<xml_diff>
--- a/Ausarbeitung/Zeitmessungen.xlsx
+++ b/Ausarbeitung/Zeitmessungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\TUM\3. Semester\ASP\Projekt\ASP-Peano\Ausarbeitung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D56711-ACA6-4F35-9E7E-0EB4D45ED48B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D5C3F3-3F2D-42C0-B9E1-CDD7FB74210C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,13 +319,13 @@
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -3006,13 +3006,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -4037,8 +4037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A4:AC31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5005,19 +5005,19 @@
         <v>29</v>
       </c>
       <c r="B22" s="12">
-        <f>C7</f>
+        <f t="shared" ref="B22:B27" si="12">C7</f>
         <v>19267.05</v>
       </c>
       <c r="C22" s="12">
-        <f t="shared" ref="C22:E22" si="12">D7</f>
+        <f t="shared" ref="C22:E22" si="13">D7</f>
         <v>22095.599999999999</v>
       </c>
       <c r="D22" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29450.1</v>
       </c>
       <c r="E22" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>20101.400000000001</v>
       </c>
     </row>
@@ -5025,19 +5025,19 @@
       <c r="A23" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="28">
-        <f>C8</f>
+      <c r="B23" s="26">
+        <f t="shared" si="12"/>
         <v>207927.45</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="26">
         <f>D8</f>
         <v>221833.05</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="26">
         <f>E8</f>
         <v>252268.05</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="26">
         <f>F8</f>
         <v>212634.7</v>
       </c>
@@ -5046,20 +5046,20 @@
       <c r="A24" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="28">
-        <f>C9</f>
+      <c r="B24" s="26">
+        <f t="shared" si="12"/>
         <v>1852378.45</v>
       </c>
-      <c r="C24" s="28">
-        <f t="shared" ref="C24:E24" si="13">D9</f>
+      <c r="C24" s="26">
+        <f t="shared" ref="C24:E24" si="14">D9</f>
         <v>2074699.9</v>
       </c>
-      <c r="D24" s="28">
-        <f t="shared" si="13"/>
+      <c r="D24" s="26">
+        <f t="shared" si="14"/>
         <v>2107929.7999999998</v>
       </c>
-      <c r="E24" s="28">
-        <f t="shared" si="13"/>
+      <c r="E24" s="26">
+        <f t="shared" si="14"/>
         <v>1965193.05</v>
       </c>
     </row>
@@ -5067,19 +5067,19 @@
       <c r="A25" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="28">
-        <f>C10</f>
+      <c r="B25" s="26">
+        <f t="shared" si="12"/>
         <v>5997884.7999999998</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="26">
         <f>D10</f>
         <v>6308944.3499999996</v>
       </c>
-      <c r="D25" s="28">
+      <c r="D25" s="26">
         <f>E10</f>
         <v>6692878.8499999996</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25" s="26">
         <f>F10</f>
         <v>6039483.0499999998</v>
       </c>
@@ -5088,20 +5088,20 @@
       <c r="A26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="28">
-        <f>C11</f>
+      <c r="B26" s="26">
+        <f t="shared" si="12"/>
         <v>32001060.100000001</v>
       </c>
-      <c r="C26" s="28">
-        <f t="shared" ref="C26:E26" si="14">D11</f>
+      <c r="C26" s="26">
+        <f t="shared" ref="C26:E26" si="15">D11</f>
         <v>35985537.649999999</v>
       </c>
-      <c r="D26" s="28">
-        <f t="shared" si="14"/>
+      <c r="D26" s="26">
+        <f t="shared" si="15"/>
         <v>42620818.299999997</v>
       </c>
-      <c r="E26" s="28">
-        <f t="shared" si="14"/>
+      <c r="E26" s="26">
+        <f t="shared" si="15"/>
         <v>32756551.050000001</v>
       </c>
     </row>
@@ -5109,20 +5109,20 @@
       <c r="A27" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="28">
-        <f>C12</f>
+      <c r="B27" s="26">
+        <f t="shared" si="12"/>
         <v>264060050</v>
       </c>
-      <c r="C27" s="28">
-        <f t="shared" ref="C27:E27" si="15">D12</f>
+      <c r="C27" s="26">
+        <f t="shared" ref="C27:E27" si="16">D12</f>
         <v>276779550</v>
       </c>
-      <c r="D27" s="28">
-        <f t="shared" si="15"/>
+      <c r="D27" s="26">
+        <f t="shared" si="16"/>
         <v>303332699.99999994</v>
       </c>
-      <c r="E27" s="28">
-        <f t="shared" si="15"/>
+      <c r="E27" s="26">
+        <f t="shared" si="16"/>
         <v>260258349.99999997</v>
       </c>
     </row>
@@ -5174,13 +5174,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -6024,13 +6024,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -6874,13 +6874,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -7725,13 +7725,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -8576,13 +8576,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -9429,13 +9429,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -10284,13 +10284,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -11115,8 +11115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="Y36" sqref="Y36"/>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11137,16 +11137,17 @@
     <col min="16" max="16" width="12.5703125" style="1" customWidth="1"/>
     <col min="17" max="17" width="9.85546875" style="1" customWidth="1"/>
     <col min="21" max="21" width="10.5703125" style="4"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">

</xml_diff>